<commit_message>
some mods to workbooks
</commit_message>
<xml_diff>
--- a/CH_020314_C.xlsx
+++ b/CH_020314_C.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="135" windowWidth="25605" windowHeight="16065" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="1185" yWindow="135" windowWidth="25605" windowHeight="16065" tabRatio="626" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="152">
   <si>
     <t>Mouse ID</t>
   </si>
@@ -150,6 +150,339 @@
   </si>
   <si>
     <t>AAV_CAGGS_floxed_ChR2_tdTomato injected into V1. 100nl of virus injected at 25 nl/min. Depth = 310 um. Location = 2.56 mm left of lambda. I tested the injection pipet before injecting (and after), but for the following mouse, when I check using a flow rate of 25 nl/min, nothing came out. This means that 25 nl/min may be too slow!</t>
+  </si>
+  <si>
+    <t>2014_02_18_0000</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>LED 405 pulses. AS closed. At soma. Good evoked epsps.</t>
+  </si>
+  <si>
+    <t>2014_02_18_0001</t>
+  </si>
+  <si>
+    <t>LED 405 pulses. AS closed. At axon tract below L6. No evoked PSPs</t>
+  </si>
+  <si>
+    <t>2014_02_18_0002</t>
+  </si>
+  <si>
+    <t>LED 470 pulses. AS closed. At axon tract below L6 No evoked potentials.</t>
+  </si>
+  <si>
+    <t>2014_02_18_0003</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>IV curve. Cell at [-250 -285]</t>
+  </si>
+  <si>
+    <t>2014_02_18_0004</t>
+  </si>
+  <si>
+    <t>LED 405 nm steps. No evoked response. AS closed. Vhold = -60. At soma</t>
+  </si>
+  <si>
+    <t>2014_02_18_0005</t>
+  </si>
+  <si>
+    <t>LED 470 nm steps. Decent evoked response. AS closed. Vhold = -60. At soma</t>
+  </si>
+  <si>
+    <t>2014_02_18_0006</t>
+  </si>
+  <si>
+    <t>LED 590 nm steps. No evoked response. AS closed. Vhold = -60. At soma</t>
+  </si>
+  <si>
+    <t>2014_02_18_0008</t>
+  </si>
+  <si>
+    <t>LED 470 nm steps. NO response. AS closed. Vhold = -60. At axon tract below L6. Axon tract at [-590, -616]</t>
+  </si>
+  <si>
+    <t>2014_02_18_0009</t>
+  </si>
+  <si>
+    <t>LED 470 nm steps. No evoked response. AS closed. Vhold = -60. At axon tract below L6. Axon tract at [-590, -616]. This time I used only 10 volt modulations of different pulse lengths, from 2ms to about 45 ms.</t>
+  </si>
+  <si>
+    <t>2014_02_18_0010</t>
+  </si>
+  <si>
+    <t>LED 470 nm steps with AS open. Vhold = -60. At axon tract below L6. Axon tract at [-590, -616]. This time I used only 10 volt modulations of different pulse lengths, from 2ms to about 45 ms. There may have been an inhibitory current activated by the light onset.</t>
+  </si>
+  <si>
+    <t>2014_02_18_0011</t>
+  </si>
+  <si>
+    <t>LED 470 nm steps with AS open. Vhold = -85. At axon tract below L6. Axon tract at [-590, -616]. This time I used only 10 volt modulations of different pulse lengths, from 2ms to about 45 ms. Holding the cell at Cl- Erev may have uncovered an excitatory current for shorter pulses. Longer pulses my make the synapses clam up...</t>
+  </si>
+  <si>
+    <t>2014_02_18_0012</t>
+  </si>
+  <si>
+    <t>LED 470 nm short pulses at the axon tract with the AS closed. Vhold = -85. No noticeable response…</t>
+  </si>
+  <si>
+    <t>2014_02_18_0014</t>
+  </si>
+  <si>
+    <t>LED 470 nm pulses, AS closed, at axon tract. Pulse witdth was variable. Vhold = -85. No obvious response</t>
+  </si>
+  <si>
+    <t>2014_02_18_0015</t>
+  </si>
+  <si>
+    <t>LED 470 nm pulses, AS closed, at axon tract, but more medial than the first location. Vhold = -85. No obvious response</t>
+  </si>
+  <si>
+    <t>2014_02_18_0016</t>
+  </si>
+  <si>
+    <t>LED 470 nm pulses, AS open. At soma.Vold = -85. Big responses, but I'm loosing the cell.</t>
+  </si>
+  <si>
+    <t>2014_02_18_0017</t>
+  </si>
+  <si>
+    <t>LED 470 nm pulses, AS open. At soma.Vold = 0. Big responses.</t>
+  </si>
+  <si>
+    <t>2014_02_18_0018</t>
+  </si>
+  <si>
+    <t>LED 470 nm 10 Hz train. AS open. At soma.Vold = -60.</t>
+  </si>
+  <si>
+    <t>2014_02_18_0019</t>
+  </si>
+  <si>
+    <t>LED 470 nm 10 Hz train. AS open. At soma.Vold = 0.</t>
+  </si>
+  <si>
+    <t>2014_02_18_0020</t>
+  </si>
+  <si>
+    <t>LED 470 nm 20 Hz train. AS open. At soma.Vold = 0.</t>
+  </si>
+  <si>
+    <t>2014_02_18_0021</t>
+  </si>
+  <si>
+    <t>LED 470 nm 40 Hz train. AS open. At soma.Vold = 0.</t>
+  </si>
+  <si>
+    <t>2014_02_18_0022</t>
+  </si>
+  <si>
+    <t>LED 470 nm 40 Hz train. AS open. At soma.Vold = -60mv</t>
+  </si>
+  <si>
+    <t>2014_02_18_0023</t>
+  </si>
+  <si>
+    <t>LED 470 nm 40 Hz train. AS open. At soma.Vold = -85mv. Lost the cell on the last sweep, but interesting depression I'm fairly certain.</t>
+  </si>
+  <si>
+    <t>out</t>
+  </si>
+  <si>
+    <t>Vout = 2 mV. Pictures of cell on crash. Cell was about 680 um from pia.</t>
+  </si>
+  <si>
+    <t>2014_02_18_0024</t>
+  </si>
+  <si>
+    <t>IV curve. Bridge balance off?</t>
+  </si>
+  <si>
+    <t>2014_02_18_0025</t>
+  </si>
+  <si>
+    <t>IV curve. Bridge balance off? Larver amplitude current pulses. With spiking.</t>
+  </si>
+  <si>
+    <t>2014_02_18_0028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED 470 nm steps. Very responsive at 0.8 volts. </t>
+  </si>
+  <si>
+    <t>2014_02_18_0029</t>
+  </si>
+  <si>
+    <t>LED 470 trains at 10 Hz. AS open. Vhold  = -85</t>
+  </si>
+  <si>
+    <t>2014_02_18_0030</t>
+  </si>
+  <si>
+    <t>LED 470 trains at 20 Hz. AS open. Vhold  = -85</t>
+  </si>
+  <si>
+    <t>2014_02_18_0032</t>
+  </si>
+  <si>
+    <t>LED 470 trains at 40 Hz. AS open. Vhold  = -85</t>
+  </si>
+  <si>
+    <t>2014_02_18_0033</t>
+  </si>
+  <si>
+    <t>LED 470 trains at 5 Hz. AS open. Vhold  = -85</t>
+  </si>
+  <si>
+    <t>2014_02_18_0034</t>
+  </si>
+  <si>
+    <t>LED 470 trains at 5 Hz. AS open. Vhold  = 0 mV</t>
+  </si>
+  <si>
+    <t>2014_02_18_0035</t>
+  </si>
+  <si>
+    <t>LED 470 trains at 40 Hz. AS open. Vhold  = 0 mV</t>
+  </si>
+  <si>
+    <t>2014_02_18_0036</t>
+  </si>
+  <si>
+    <t>LED 470 trains at 10 Hz. AS open. Vhold  = 0 mV</t>
+  </si>
+  <si>
+    <t>2014_02_18_0037</t>
+  </si>
+  <si>
+    <t>LED 470 trains at 20 Hz. AS open. Vhold  = 0 mV</t>
+  </si>
+  <si>
+    <t>2014_02_18_0038</t>
+  </si>
+  <si>
+    <t>LED 470 trains at 20 Hz. AS open. Vhold  = -60 mV</t>
+  </si>
+  <si>
+    <t>2014_02_18_0039</t>
+  </si>
+  <si>
+    <t>LED 470 trains at 10 Hz. AS open. Vhold  = -60 mV</t>
+  </si>
+  <si>
+    <t>2014_02_18_0040</t>
+  </si>
+  <si>
+    <t>LED 470 trains at 40 Hz. AS open. Vhold  = -60 mV</t>
+  </si>
+  <si>
+    <t>2014_02_18_0041</t>
+  </si>
+  <si>
+    <t>LED 470 trains at 5 Hz. AS open. Vhold  = -60 mV</t>
+  </si>
+  <si>
+    <t>Vout = 5 mV. Cell was about 360 um from the pia. Pictures on crash.</t>
+  </si>
+  <si>
+    <t>2014_02_18_0042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IV curve. </t>
+  </si>
+  <si>
+    <t>2014_02_18_0043</t>
+  </si>
+  <si>
+    <t>LED 470 nm steps. Good response at 2.5 Volts. Vhold = -60???</t>
+  </si>
+  <si>
+    <t>2014_02_18_0044</t>
+  </si>
+  <si>
+    <t>LED 470 trains at 5 Hz. Vhold  = -85 mV</t>
+  </si>
+  <si>
+    <t>2014_02_18_0045</t>
+  </si>
+  <si>
+    <t>LED 470 trains at 20 Hz. Vhold  = -85 mV</t>
+  </si>
+  <si>
+    <t>2014_02_18_0046</t>
+  </si>
+  <si>
+    <t>LED 470 trains at 10 Hz. Vhold  = -85 mV</t>
+  </si>
+  <si>
+    <t>2014_02_18_0047</t>
+  </si>
+  <si>
+    <t>LED 470 trains at 40 Hz. Vhold  = -85 mV</t>
+  </si>
+  <si>
+    <t>2014_02_18_0048</t>
+  </si>
+  <si>
+    <t>LED 470 trains at 40 Hz. Vhold  = 0 mV</t>
+  </si>
+  <si>
+    <t>2014_02_18_0049</t>
+  </si>
+  <si>
+    <t>LED 470 trains at 5 Hz. Vhold  = 0 mV</t>
+  </si>
+  <si>
+    <t>2014_02_18_0050</t>
+  </si>
+  <si>
+    <t>LED 470 trains at 20 Hz. Vhold  = 0 mV</t>
+  </si>
+  <si>
+    <t>2014_02_18_0051</t>
+  </si>
+  <si>
+    <t>LED 470 trains at 10 Hz. Vhold  = 0 mV</t>
+  </si>
+  <si>
+    <t>2014_02_18_0052</t>
+  </si>
+  <si>
+    <t>LED 470 steps Vhold  = 0 mV</t>
+  </si>
+  <si>
+    <t>2014_02_18_0053</t>
+  </si>
+  <si>
+    <t>LED 470 steps Vhold  = -60 mV</t>
+  </si>
+  <si>
+    <t>2014_02_18_0054</t>
+  </si>
+  <si>
+    <t>LED 470 steps Vhold  = -85 mV Cell died on last sweep.</t>
+  </si>
+  <si>
+    <t>2014_02_18_0055</t>
+  </si>
+  <si>
+    <t>Vout = 4 mV, Cell was about 450 um from pia.</t>
+  </si>
+  <si>
+    <t>K Glucontate, adjusted with DI to osm</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Nice expression of ChR2. Many axon clouds to record from. I tried recording from a PY cell in an axon cloud and tried evoking responses by targeting the axon tract below L6. This did not evoke responses. The remaining cells, I just looked at the frequency dependence of synaptic depression at -85, -60, and 0mV (i.e., inhibition, excitation, and at rest).</t>
+  </si>
+  <si>
+    <t>4% PFA</t>
   </si>
 </sst>
 </file>
@@ -688,7 +1021,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -789,13 +1122,7 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -807,6 +1134,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -897,32 +1233,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1375,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="F100" sqref="F100:H100"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1393,66 +1729,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="55" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
       <c r="G1" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="22"/>
+      <c r="H1" s="22">
+        <v>297</v>
+      </c>
     </row>
     <row r="2" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="24"/>
+      <c r="H2" s="24">
+        <v>303</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="43"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="42">
+        <v>34</v>
+      </c>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="44"/>
     </row>
     <row r="4" spans="1:8" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="47"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="45" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="48"/>
     </row>
     <row r="5" spans="1:8" ht="26.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
     </row>
     <row r="6" spans="1:8" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -1470,571 +1818,1101 @@
       <c r="E6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="35"/>
-      <c r="H6" s="36"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="40"/>
     </row>
     <row r="7" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="39"/>
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="34">
+        <v>6</v>
+      </c>
+      <c r="E7" s="34"/>
+      <c r="F7" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="36"/>
+      <c r="H7" s="37"/>
     </row>
     <row r="8" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="39"/>
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="34">
+        <v>6</v>
+      </c>
+      <c r="E8" s="34"/>
+      <c r="F8" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
     </row>
     <row r="9" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="39"/>
-    </row>
-    <row r="10" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="34">
+        <v>6</v>
+      </c>
+      <c r="E9" s="34"/>
+      <c r="F9" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="36"/>
+      <c r="H9" s="37"/>
+    </row>
+    <row r="10" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="39"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="37"/>
     </row>
     <row r="11" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="39"/>
+      <c r="A11" s="3">
+        <v>2</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="34">
+        <v>6</v>
+      </c>
+      <c r="E11" s="34">
+        <v>-70</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="36"/>
+      <c r="H11" s="37"/>
     </row>
     <row r="12" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="39"/>
+      <c r="A12" s="3">
+        <v>2</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="34">
+        <v>6</v>
+      </c>
+      <c r="E12" s="34"/>
+      <c r="F12" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="36"/>
+      <c r="H12" s="37"/>
     </row>
     <row r="13" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="39"/>
+      <c r="A13" s="3">
+        <v>2</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="34">
+        <v>6</v>
+      </c>
+      <c r="E13" s="34"/>
+      <c r="F13" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="36"/>
+      <c r="H13" s="37"/>
     </row>
     <row r="14" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="39"/>
+      <c r="A14" s="3">
+        <v>2</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="34">
+        <v>6</v>
+      </c>
+      <c r="E14" s="34"/>
+      <c r="F14" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="36"/>
+      <c r="H14" s="37"/>
     </row>
     <row r="15" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="39"/>
-    </row>
-    <row r="16" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="39"/>
-    </row>
-    <row r="17" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="39"/>
-    </row>
-    <row r="18" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="39"/>
+      <c r="A15" s="3">
+        <v>2</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="34">
+        <v>6</v>
+      </c>
+      <c r="E15" s="34"/>
+      <c r="F15" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="36"/>
+      <c r="H15" s="37"/>
+    </row>
+    <row r="16" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>2</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="34">
+        <v>6</v>
+      </c>
+      <c r="E16" s="34"/>
+      <c r="F16" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="36"/>
+      <c r="H16" s="37"/>
+    </row>
+    <row r="17" spans="1:8" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>2</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="34">
+        <v>6</v>
+      </c>
+      <c r="E17" s="34"/>
+      <c r="F17" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="36"/>
+      <c r="H17" s="37"/>
+    </row>
+    <row r="18" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>2</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="34">
+        <v>6</v>
+      </c>
+      <c r="E18" s="34"/>
+      <c r="F18" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
     </row>
     <row r="19" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="39"/>
+      <c r="A19" s="3">
+        <v>2</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="34">
+        <v>6</v>
+      </c>
+      <c r="E19" s="34"/>
+      <c r="F19" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="36"/>
+      <c r="H19" s="37"/>
     </row>
     <row r="20" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="39"/>
-    </row>
-    <row r="21" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="39"/>
-    </row>
-    <row r="22" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="39"/>
+      <c r="A20" s="3">
+        <v>2</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="34">
+        <v>6</v>
+      </c>
+      <c r="E20" s="34"/>
+      <c r="F20" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" s="36"/>
+      <c r="H20" s="37"/>
+    </row>
+    <row r="21" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>2</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="34">
+        <v>6</v>
+      </c>
+      <c r="E21" s="34"/>
+      <c r="F21" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21" s="36"/>
+      <c r="H21" s="37"/>
+    </row>
+    <row r="22" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>2</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="34">
+        <v>6</v>
+      </c>
+      <c r="E22" s="34"/>
+      <c r="F22" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" s="36"/>
+      <c r="H22" s="37"/>
     </row>
     <row r="23" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="39"/>
+      <c r="A23" s="3">
+        <v>2</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="34">
+        <v>6</v>
+      </c>
+      <c r="E23" s="34"/>
+      <c r="F23" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" s="36"/>
+      <c r="H23" s="37"/>
     </row>
     <row r="24" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="39"/>
+      <c r="A24" s="3">
+        <v>2</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="34">
+        <v>6</v>
+      </c>
+      <c r="E24" s="34"/>
+      <c r="F24" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="G24" s="36"/>
+      <c r="H24" s="37"/>
     </row>
     <row r="25" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="39"/>
+      <c r="A25" s="3">
+        <v>2</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="34">
+        <v>6</v>
+      </c>
+      <c r="E25" s="34"/>
+      <c r="F25" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="G25" s="36"/>
+      <c r="H25" s="37"/>
     </row>
     <row r="26" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="39"/>
+      <c r="A26" s="3">
+        <v>2</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="34">
+        <v>6</v>
+      </c>
+      <c r="E26" s="34"/>
+      <c r="F26" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="G26" s="36"/>
+      <c r="H26" s="37"/>
     </row>
     <row r="27" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="39"/>
+      <c r="A27" s="3">
+        <v>2</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="34">
+        <v>6</v>
+      </c>
+      <c r="E27" s="34"/>
+      <c r="F27" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="G27" s="36"/>
+      <c r="H27" s="37"/>
     </row>
     <row r="28" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="39"/>
-    </row>
-    <row r="29" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="39"/>
+      <c r="A28" s="3">
+        <v>2</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="34">
+        <v>6</v>
+      </c>
+      <c r="E28" s="34"/>
+      <c r="F28" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="G28" s="36"/>
+      <c r="H28" s="37"/>
+    </row>
+    <row r="29" spans="1:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>2</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="34">
+        <v>6</v>
+      </c>
+      <c r="E29" s="34"/>
+      <c r="F29" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="G29" s="36"/>
+      <c r="H29" s="37"/>
     </row>
     <row r="30" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
+      <c r="A30" s="3">
+        <v>2</v>
+      </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="39"/>
-    </row>
-    <row r="31" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="34">
+        <v>6</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="F30" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="G30" s="36"/>
+      <c r="H30" s="37"/>
+    </row>
+    <row r="31" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="39"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="37"/>
     </row>
     <row r="32" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="39"/>
+      <c r="A32" s="3">
+        <v>3</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="34">
+        <v>9</v>
+      </c>
+      <c r="E32" s="34">
+        <v>-75</v>
+      </c>
+      <c r="F32" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="G32" s="36"/>
+      <c r="H32" s="37"/>
     </row>
     <row r="33" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="39"/>
+      <c r="A33" s="3">
+        <v>3</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="34">
+        <v>9</v>
+      </c>
+      <c r="E33" s="34"/>
+      <c r="F33" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="G33" s="36"/>
+      <c r="H33" s="37"/>
     </row>
     <row r="34" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="39"/>
+      <c r="A34" s="3">
+        <v>3</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="34">
+        <v>9</v>
+      </c>
+      <c r="E34" s="34"/>
+      <c r="F34" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="G34" s="36"/>
+      <c r="H34" s="37"/>
     </row>
     <row r="35" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="39"/>
+      <c r="A35" s="3">
+        <v>3</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="34">
+        <v>9</v>
+      </c>
+      <c r="E35" s="34"/>
+      <c r="F35" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="G35" s="36"/>
+      <c r="H35" s="37"/>
     </row>
     <row r="36" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="37"/>
-      <c r="G36" s="38"/>
-      <c r="H36" s="39"/>
+      <c r="A36" s="3">
+        <v>3</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="34">
+        <v>9</v>
+      </c>
+      <c r="E36" s="34"/>
+      <c r="F36" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="G36" s="36"/>
+      <c r="H36" s="37"/>
     </row>
     <row r="37" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="39"/>
+      <c r="A37" s="3">
+        <v>3</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="34">
+        <v>9</v>
+      </c>
+      <c r="E37" s="34"/>
+      <c r="F37" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="G37" s="36"/>
+      <c r="H37" s="37"/>
     </row>
     <row r="38" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="39"/>
+      <c r="A38" s="3">
+        <v>3</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="34">
+        <v>9</v>
+      </c>
+      <c r="E38" s="34"/>
+      <c r="F38" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="G38" s="36"/>
+      <c r="H38" s="37"/>
     </row>
     <row r="39" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="38"/>
-      <c r="H39" s="39"/>
+      <c r="A39" s="3">
+        <v>3</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="34">
+        <v>9</v>
+      </c>
+      <c r="E39" s="34"/>
+      <c r="F39" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="G39" s="36"/>
+      <c r="H39" s="37"/>
     </row>
     <row r="40" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="38"/>
-      <c r="H40" s="39"/>
+      <c r="A40" s="3">
+        <v>3</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="34">
+        <v>9</v>
+      </c>
+      <c r="E40" s="34"/>
+      <c r="F40" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="G40" s="36"/>
+      <c r="H40" s="37"/>
     </row>
     <row r="41" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="37"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="39"/>
+      <c r="A41" s="3">
+        <v>3</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="34">
+        <v>9</v>
+      </c>
+      <c r="E41" s="34"/>
+      <c r="F41" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="G41" s="36"/>
+      <c r="H41" s="37"/>
     </row>
     <row r="42" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="38"/>
-      <c r="H42" s="39"/>
+      <c r="A42" s="3">
+        <v>3</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="34">
+        <v>9</v>
+      </c>
+      <c r="E42" s="34"/>
+      <c r="F42" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="G42" s="36"/>
+      <c r="H42" s="37"/>
     </row>
     <row r="43" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="38"/>
-      <c r="H43" s="39"/>
+      <c r="A43" s="3">
+        <v>3</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="34">
+        <v>9</v>
+      </c>
+      <c r="E43" s="34"/>
+      <c r="F43" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="G43" s="36"/>
+      <c r="H43" s="37"/>
     </row>
     <row r="44" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="38"/>
-      <c r="H44" s="39"/>
+      <c r="A44" s="3">
+        <v>3</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" s="34">
+        <v>9</v>
+      </c>
+      <c r="E44" s="34"/>
+      <c r="F44" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="G44" s="36"/>
+      <c r="H44" s="37"/>
     </row>
     <row r="45" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="37"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="39"/>
+      <c r="A45" s="3">
+        <v>3</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D45" s="34">
+        <v>9</v>
+      </c>
+      <c r="E45" s="34"/>
+      <c r="F45" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="G45" s="36"/>
+      <c r="H45" s="37"/>
     </row>
     <row r="46" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="37"/>
-      <c r="G46" s="38"/>
-      <c r="H46" s="39"/>
+      <c r="A46" s="3">
+        <v>3</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D46" s="34">
+        <v>9</v>
+      </c>
+      <c r="E46" s="34"/>
+      <c r="F46" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="G46" s="36"/>
+      <c r="H46" s="37"/>
     </row>
     <row r="47" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
+      <c r="A47" s="3">
+        <v>3</v>
+      </c>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="23"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="38"/>
-      <c r="H47" s="39"/>
-    </row>
-    <row r="48" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D47" s="34"/>
+      <c r="E47" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="F47" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="G47" s="36"/>
+      <c r="H47" s="37"/>
+    </row>
+    <row r="48" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="37"/>
-      <c r="G48" s="38"/>
-      <c r="H48" s="39"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="35"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="37"/>
     </row>
     <row r="49" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="37"/>
-      <c r="G49" s="38"/>
-      <c r="H49" s="39"/>
+      <c r="A49" s="3">
+        <v>4</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" s="34">
+        <v>9</v>
+      </c>
+      <c r="E49" s="34">
+        <v>-65</v>
+      </c>
+      <c r="F49" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="G49" s="36"/>
+      <c r="H49" s="37"/>
     </row>
     <row r="50" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="38"/>
-      <c r="H50" s="39"/>
+      <c r="A50" s="3">
+        <v>4</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D50" s="34">
+        <v>9</v>
+      </c>
+      <c r="E50" s="34"/>
+      <c r="F50" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="G50" s="36"/>
+      <c r="H50" s="37"/>
     </row>
     <row r="51" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="23"/>
-      <c r="F51" s="37"/>
-      <c r="G51" s="38"/>
-      <c r="H51" s="39"/>
+      <c r="A51" s="3">
+        <v>4</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D51" s="34">
+        <v>9</v>
+      </c>
+      <c r="E51" s="34"/>
+      <c r="F51" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="G51" s="36"/>
+      <c r="H51" s="37"/>
     </row>
     <row r="52" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="37"/>
-      <c r="G52" s="38"/>
-      <c r="H52" s="39"/>
+      <c r="A52" s="3">
+        <v>4</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D52" s="34">
+        <v>9</v>
+      </c>
+      <c r="E52" s="34"/>
+      <c r="F52" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="G52" s="36"/>
+      <c r="H52" s="37"/>
     </row>
     <row r="53" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="23"/>
-      <c r="F53" s="37"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="39"/>
+      <c r="A53" s="3">
+        <v>4</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D53" s="34">
+        <v>9</v>
+      </c>
+      <c r="E53" s="34"/>
+      <c r="F53" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="G53" s="36"/>
+      <c r="H53" s="37"/>
     </row>
     <row r="54" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="23"/>
-      <c r="F54" s="37"/>
-      <c r="G54" s="38"/>
-      <c r="H54" s="39"/>
+      <c r="A54" s="3">
+        <v>4</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54" s="34">
+        <v>9</v>
+      </c>
+      <c r="E54" s="34"/>
+      <c r="F54" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="G54" s="36"/>
+      <c r="H54" s="37"/>
     </row>
     <row r="55" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="23"/>
-      <c r="F55" s="37"/>
-      <c r="G55" s="38"/>
-      <c r="H55" s="39"/>
+      <c r="A55" s="3">
+        <v>4</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D55" s="34">
+        <v>9</v>
+      </c>
+      <c r="E55" s="34"/>
+      <c r="F55" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="G55" s="36"/>
+      <c r="H55" s="37"/>
     </row>
     <row r="56" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="23"/>
-      <c r="F56" s="37"/>
-      <c r="G56" s="38"/>
-      <c r="H56" s="39"/>
+      <c r="A56" s="3">
+        <v>4</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D56" s="34">
+        <v>9</v>
+      </c>
+      <c r="E56" s="34"/>
+      <c r="F56" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="G56" s="36"/>
+      <c r="H56" s="37"/>
     </row>
     <row r="57" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="23"/>
-      <c r="F57" s="37"/>
-      <c r="G57" s="38"/>
-      <c r="H57" s="39"/>
+      <c r="A57" s="3">
+        <v>4</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D57" s="34">
+        <v>9</v>
+      </c>
+      <c r="E57" s="34"/>
+      <c r="F57" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="G57" s="36"/>
+      <c r="H57" s="37"/>
     </row>
     <row r="58" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="3"/>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="23"/>
-      <c r="F58" s="37"/>
-      <c r="G58" s="38"/>
-      <c r="H58" s="39"/>
+      <c r="A58" s="3">
+        <v>4</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D58" s="34">
+        <v>9</v>
+      </c>
+      <c r="E58" s="34"/>
+      <c r="F58" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="G58" s="36"/>
+      <c r="H58" s="37"/>
     </row>
     <row r="59" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="3"/>
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="23"/>
-      <c r="F59" s="37"/>
-      <c r="G59" s="38"/>
-      <c r="H59" s="39"/>
+      <c r="A59" s="3">
+        <v>4</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D59" s="34">
+        <v>9</v>
+      </c>
+      <c r="E59" s="34"/>
+      <c r="F59" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="G59" s="36"/>
+      <c r="H59" s="37"/>
     </row>
     <row r="60" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="3"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="23"/>
-      <c r="F60" s="37"/>
-      <c r="G60" s="38"/>
-      <c r="H60" s="39"/>
+      <c r="A60" s="3">
+        <v>4</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D60" s="34">
+        <v>9</v>
+      </c>
+      <c r="E60" s="34"/>
+      <c r="F60" s="35" t="s">
+        <v>143</v>
+      </c>
+      <c r="G60" s="36"/>
+      <c r="H60" s="37"/>
     </row>
     <row r="61" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="23"/>
-      <c r="F61" s="37"/>
-      <c r="G61" s="38"/>
-      <c r="H61" s="39"/>
+      <c r="A61" s="3">
+        <v>4</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D61" s="34">
+        <v>9</v>
+      </c>
+      <c r="E61" s="34"/>
+      <c r="F61" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="G61" s="36"/>
+      <c r="H61" s="37"/>
     </row>
     <row r="62" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="3"/>
-      <c r="B62" s="4"/>
+      <c r="A62" s="3">
+        <v>4</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>146</v>
+      </c>
       <c r="C62" s="4"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="23"/>
-      <c r="F62" s="37"/>
-      <c r="G62" s="38"/>
-      <c r="H62" s="39"/>
+      <c r="D62" s="34">
+        <v>9</v>
+      </c>
+      <c r="E62" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="F62" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="G62" s="36"/>
+      <c r="H62" s="37"/>
     </row>
     <row r="63" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
@@ -2042,9 +2920,9 @@
       <c r="C63" s="4"/>
       <c r="D63" s="5"/>
       <c r="E63" s="23"/>
-      <c r="F63" s="37"/>
-      <c r="G63" s="38"/>
-      <c r="H63" s="39"/>
+      <c r="F63" s="35"/>
+      <c r="G63" s="36"/>
+      <c r="H63" s="37"/>
     </row>
     <row r="64" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
@@ -2052,9 +2930,9 @@
       <c r="C64" s="4"/>
       <c r="D64" s="5"/>
       <c r="E64" s="23"/>
-      <c r="F64" s="37"/>
-      <c r="G64" s="38"/>
-      <c r="H64" s="39"/>
+      <c r="F64" s="35"/>
+      <c r="G64" s="36"/>
+      <c r="H64" s="37"/>
     </row>
     <row r="65" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
@@ -2062,9 +2940,9 @@
       <c r="C65" s="4"/>
       <c r="D65" s="5"/>
       <c r="E65" s="23"/>
-      <c r="F65" s="37"/>
-      <c r="G65" s="38"/>
-      <c r="H65" s="39"/>
+      <c r="F65" s="35"/>
+      <c r="G65" s="36"/>
+      <c r="H65" s="37"/>
     </row>
     <row r="66" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
@@ -2072,9 +2950,9 @@
       <c r="C66" s="4"/>
       <c r="D66" s="5"/>
       <c r="E66" s="23"/>
-      <c r="F66" s="37"/>
-      <c r="G66" s="38"/>
-      <c r="H66" s="39"/>
+      <c r="F66" s="35"/>
+      <c r="G66" s="36"/>
+      <c r="H66" s="37"/>
     </row>
     <row r="67" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
@@ -2082,9 +2960,9 @@
       <c r="C67" s="4"/>
       <c r="D67" s="5"/>
       <c r="E67" s="23"/>
-      <c r="F67" s="37"/>
-      <c r="G67" s="38"/>
-      <c r="H67" s="39"/>
+      <c r="F67" s="35"/>
+      <c r="G67" s="36"/>
+      <c r="H67" s="37"/>
     </row>
     <row r="68" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
@@ -2092,9 +2970,9 @@
       <c r="C68" s="4"/>
       <c r="D68" s="5"/>
       <c r="E68" s="23"/>
-      <c r="F68" s="37"/>
-      <c r="G68" s="38"/>
-      <c r="H68" s="39"/>
+      <c r="F68" s="35"/>
+      <c r="G68" s="36"/>
+      <c r="H68" s="37"/>
     </row>
     <row r="69" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
@@ -2102,9 +2980,9 @@
       <c r="C69" s="4"/>
       <c r="D69" s="5"/>
       <c r="E69" s="23"/>
-      <c r="F69" s="37"/>
-      <c r="G69" s="38"/>
-      <c r="H69" s="39"/>
+      <c r="F69" s="35"/>
+      <c r="G69" s="36"/>
+      <c r="H69" s="37"/>
     </row>
     <row r="70" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
@@ -2112,9 +2990,9 @@
       <c r="C70" s="4"/>
       <c r="D70" s="5"/>
       <c r="E70" s="23"/>
-      <c r="F70" s="37"/>
-      <c r="G70" s="38"/>
-      <c r="H70" s="39"/>
+      <c r="F70" s="35"/>
+      <c r="G70" s="36"/>
+      <c r="H70" s="37"/>
     </row>
     <row r="71" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
@@ -2122,9 +3000,9 @@
       <c r="C71" s="4"/>
       <c r="D71" s="5"/>
       <c r="E71" s="23"/>
-      <c r="F71" s="37"/>
-      <c r="G71" s="38"/>
-      <c r="H71" s="39"/>
+      <c r="F71" s="35"/>
+      <c r="G71" s="36"/>
+      <c r="H71" s="37"/>
     </row>
     <row r="72" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
@@ -2132,9 +3010,9 @@
       <c r="C72" s="4"/>
       <c r="D72" s="5"/>
       <c r="E72" s="23"/>
-      <c r="F72" s="37"/>
-      <c r="G72" s="38"/>
-      <c r="H72" s="39"/>
+      <c r="F72" s="35"/>
+      <c r="G72" s="36"/>
+      <c r="H72" s="37"/>
     </row>
     <row r="73" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
@@ -2142,9 +3020,9 @@
       <c r="C73" s="4"/>
       <c r="D73" s="5"/>
       <c r="E73" s="23"/>
-      <c r="F73" s="37"/>
-      <c r="G73" s="38"/>
-      <c r="H73" s="39"/>
+      <c r="F73" s="35"/>
+      <c r="G73" s="36"/>
+      <c r="H73" s="37"/>
     </row>
     <row r="74" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
@@ -2152,9 +3030,9 @@
       <c r="C74" s="4"/>
       <c r="D74" s="5"/>
       <c r="E74" s="23"/>
-      <c r="F74" s="37"/>
-      <c r="G74" s="38"/>
-      <c r="H74" s="39"/>
+      <c r="F74" s="35"/>
+      <c r="G74" s="36"/>
+      <c r="H74" s="37"/>
     </row>
     <row r="75" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
@@ -2162,9 +3040,9 @@
       <c r="C75" s="4"/>
       <c r="D75" s="5"/>
       <c r="E75" s="23"/>
-      <c r="F75" s="37"/>
-      <c r="G75" s="38"/>
-      <c r="H75" s="39"/>
+      <c r="F75" s="35"/>
+      <c r="G75" s="36"/>
+      <c r="H75" s="37"/>
     </row>
     <row r="76" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
@@ -2172,9 +3050,9 @@
       <c r="C76" s="4"/>
       <c r="D76" s="5"/>
       <c r="E76" s="23"/>
-      <c r="F76" s="37"/>
-      <c r="G76" s="38"/>
-      <c r="H76" s="39"/>
+      <c r="F76" s="35"/>
+      <c r="G76" s="36"/>
+      <c r="H76" s="37"/>
     </row>
     <row r="77" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
@@ -2182,9 +3060,9 @@
       <c r="C77" s="4"/>
       <c r="D77" s="5"/>
       <c r="E77" s="23"/>
-      <c r="F77" s="37"/>
-      <c r="G77" s="38"/>
-      <c r="H77" s="39"/>
+      <c r="F77" s="35"/>
+      <c r="G77" s="36"/>
+      <c r="H77" s="37"/>
     </row>
     <row r="78" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
@@ -2192,9 +3070,9 @@
       <c r="C78" s="4"/>
       <c r="D78" s="5"/>
       <c r="E78" s="23"/>
-      <c r="F78" s="37"/>
-      <c r="G78" s="38"/>
-      <c r="H78" s="39"/>
+      <c r="F78" s="35"/>
+      <c r="G78" s="36"/>
+      <c r="H78" s="37"/>
     </row>
     <row r="79" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
@@ -2202,9 +3080,9 @@
       <c r="C79" s="4"/>
       <c r="D79" s="5"/>
       <c r="E79" s="23"/>
-      <c r="F79" s="37"/>
-      <c r="G79" s="38"/>
-      <c r="H79" s="39"/>
+      <c r="F79" s="35"/>
+      <c r="G79" s="36"/>
+      <c r="H79" s="37"/>
     </row>
     <row r="80" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
@@ -2212,9 +3090,9 @@
       <c r="C80" s="4"/>
       <c r="D80" s="5"/>
       <c r="E80" s="23"/>
-      <c r="F80" s="37"/>
-      <c r="G80" s="38"/>
-      <c r="H80" s="39"/>
+      <c r="F80" s="35"/>
+      <c r="G80" s="36"/>
+      <c r="H80" s="37"/>
     </row>
     <row r="81" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
@@ -2222,9 +3100,9 @@
       <c r="C81" s="4"/>
       <c r="D81" s="5"/>
       <c r="E81" s="23"/>
-      <c r="F81" s="37"/>
-      <c r="G81" s="38"/>
-      <c r="H81" s="39"/>
+      <c r="F81" s="35"/>
+      <c r="G81" s="36"/>
+      <c r="H81" s="37"/>
     </row>
     <row r="82" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
@@ -2232,9 +3110,9 @@
       <c r="C82" s="4"/>
       <c r="D82" s="5"/>
       <c r="E82" s="23"/>
-      <c r="F82" s="37"/>
-      <c r="G82" s="38"/>
-      <c r="H82" s="39"/>
+      <c r="F82" s="35"/>
+      <c r="G82" s="36"/>
+      <c r="H82" s="37"/>
     </row>
     <row r="83" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
@@ -2242,9 +3120,9 @@
       <c r="C83" s="4"/>
       <c r="D83" s="5"/>
       <c r="E83" s="23"/>
-      <c r="F83" s="37"/>
-      <c r="G83" s="38"/>
-      <c r="H83" s="39"/>
+      <c r="F83" s="35"/>
+      <c r="G83" s="36"/>
+      <c r="H83" s="37"/>
     </row>
     <row r="84" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
@@ -2252,9 +3130,9 @@
       <c r="C84" s="4"/>
       <c r="D84" s="5"/>
       <c r="E84" s="23"/>
-      <c r="F84" s="37"/>
-      <c r="G84" s="38"/>
-      <c r="H84" s="39"/>
+      <c r="F84" s="35"/>
+      <c r="G84" s="36"/>
+      <c r="H84" s="37"/>
     </row>
     <row r="85" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
@@ -2262,9 +3140,9 @@
       <c r="C85" s="4"/>
       <c r="D85" s="5"/>
       <c r="E85" s="23"/>
-      <c r="F85" s="37"/>
-      <c r="G85" s="38"/>
-      <c r="H85" s="39"/>
+      <c r="F85" s="35"/>
+      <c r="G85" s="36"/>
+      <c r="H85" s="37"/>
     </row>
     <row r="86" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
@@ -2272,9 +3150,9 @@
       <c r="C86" s="4"/>
       <c r="D86" s="5"/>
       <c r="E86" s="23"/>
-      <c r="F86" s="37"/>
-      <c r="G86" s="38"/>
-      <c r="H86" s="39"/>
+      <c r="F86" s="35"/>
+      <c r="G86" s="36"/>
+      <c r="H86" s="37"/>
     </row>
     <row r="87" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
@@ -2282,9 +3160,9 @@
       <c r="C87" s="4"/>
       <c r="D87" s="5"/>
       <c r="E87" s="23"/>
-      <c r="F87" s="37"/>
-      <c r="G87" s="38"/>
-      <c r="H87" s="39"/>
+      <c r="F87" s="35"/>
+      <c r="G87" s="36"/>
+      <c r="H87" s="37"/>
     </row>
     <row r="88" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
@@ -2292,9 +3170,9 @@
       <c r="C88" s="4"/>
       <c r="D88" s="5"/>
       <c r="E88" s="23"/>
-      <c r="F88" s="37"/>
-      <c r="G88" s="38"/>
-      <c r="H88" s="39"/>
+      <c r="F88" s="35"/>
+      <c r="G88" s="36"/>
+      <c r="H88" s="37"/>
     </row>
     <row r="89" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
@@ -2302,9 +3180,9 @@
       <c r="C89" s="4"/>
       <c r="D89" s="5"/>
       <c r="E89" s="23"/>
-      <c r="F89" s="37"/>
-      <c r="G89" s="38"/>
-      <c r="H89" s="39"/>
+      <c r="F89" s="35"/>
+      <c r="G89" s="36"/>
+      <c r="H89" s="37"/>
     </row>
     <row r="90" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
@@ -2312,9 +3190,9 @@
       <c r="C90" s="4"/>
       <c r="D90" s="5"/>
       <c r="E90" s="23"/>
-      <c r="F90" s="37"/>
-      <c r="G90" s="38"/>
-      <c r="H90" s="39"/>
+      <c r="F90" s="35"/>
+      <c r="G90" s="36"/>
+      <c r="H90" s="37"/>
     </row>
     <row r="91" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
@@ -2322,9 +3200,9 @@
       <c r="C91" s="4"/>
       <c r="D91" s="5"/>
       <c r="E91" s="23"/>
-      <c r="F91" s="37"/>
-      <c r="G91" s="38"/>
-      <c r="H91" s="39"/>
+      <c r="F91" s="35"/>
+      <c r="G91" s="36"/>
+      <c r="H91" s="37"/>
     </row>
     <row r="92" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
@@ -2332,9 +3210,9 @@
       <c r="C92" s="4"/>
       <c r="D92" s="5"/>
       <c r="E92" s="23"/>
-      <c r="F92" s="37"/>
-      <c r="G92" s="38"/>
-      <c r="H92" s="39"/>
+      <c r="F92" s="35"/>
+      <c r="G92" s="36"/>
+      <c r="H92" s="37"/>
     </row>
     <row r="93" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
@@ -2342,9 +3220,9 @@
       <c r="C93" s="4"/>
       <c r="D93" s="5"/>
       <c r="E93" s="23"/>
-      <c r="F93" s="37"/>
-      <c r="G93" s="38"/>
-      <c r="H93" s="39"/>
+      <c r="F93" s="35"/>
+      <c r="G93" s="36"/>
+      <c r="H93" s="37"/>
     </row>
     <row r="94" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
@@ -2352,9 +3230,9 @@
       <c r="C94" s="4"/>
       <c r="D94" s="5"/>
       <c r="E94" s="23"/>
-      <c r="F94" s="37"/>
-      <c r="G94" s="38"/>
-      <c r="H94" s="39"/>
+      <c r="F94" s="35"/>
+      <c r="G94" s="36"/>
+      <c r="H94" s="37"/>
     </row>
     <row r="95" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
@@ -2362,9 +3240,9 @@
       <c r="C95" s="4"/>
       <c r="D95" s="5"/>
       <c r="E95" s="23"/>
-      <c r="F95" s="37"/>
-      <c r="G95" s="38"/>
-      <c r="H95" s="39"/>
+      <c r="F95" s="35"/>
+      <c r="G95" s="36"/>
+      <c r="H95" s="37"/>
     </row>
     <row r="96" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
@@ -2372,9 +3250,9 @@
       <c r="C96" s="4"/>
       <c r="D96" s="5"/>
       <c r="E96" s="23"/>
-      <c r="F96" s="37"/>
-      <c r="G96" s="38"/>
-      <c r="H96" s="39"/>
+      <c r="F96" s="35"/>
+      <c r="G96" s="36"/>
+      <c r="H96" s="37"/>
     </row>
     <row r="97" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
@@ -2382,9 +3260,9 @@
       <c r="C97" s="4"/>
       <c r="D97" s="5"/>
       <c r="E97" s="23"/>
-      <c r="F97" s="37"/>
-      <c r="G97" s="38"/>
-      <c r="H97" s="39"/>
+      <c r="F97" s="35"/>
+      <c r="G97" s="36"/>
+      <c r="H97" s="37"/>
     </row>
     <row r="98" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
@@ -2392,9 +3270,9 @@
       <c r="C98" s="4"/>
       <c r="D98" s="5"/>
       <c r="E98" s="23"/>
-      <c r="F98" s="37"/>
-      <c r="G98" s="38"/>
-      <c r="H98" s="39"/>
+      <c r="F98" s="35"/>
+      <c r="G98" s="36"/>
+      <c r="H98" s="37"/>
     </row>
     <row r="99" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
@@ -2402,9 +3280,9 @@
       <c r="C99" s="4"/>
       <c r="D99" s="5"/>
       <c r="E99" s="23"/>
-      <c r="F99" s="37"/>
-      <c r="G99" s="38"/>
-      <c r="H99" s="39"/>
+      <c r="F99" s="35"/>
+      <c r="G99" s="36"/>
+      <c r="H99" s="37"/>
     </row>
     <row r="100" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
@@ -2412,103 +3290,13 @@
       <c r="C100" s="4"/>
       <c r="D100" s="5"/>
       <c r="E100" s="23"/>
-      <c r="F100" s="37"/>
-      <c r="G100" s="38"/>
-      <c r="H100" s="39"/>
+      <c r="F100" s="35"/>
+      <c r="G100" s="36"/>
+      <c r="H100" s="37"/>
     </row>
     <row r="101" spans="1:8" ht="39" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="F96:H96"/>
-    <mergeCell ref="F97:H97"/>
-    <mergeCell ref="F98:H98"/>
-    <mergeCell ref="F99:H99"/>
-    <mergeCell ref="F100:H100"/>
-    <mergeCell ref="F91:H91"/>
-    <mergeCell ref="F92:H92"/>
-    <mergeCell ref="F93:H93"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="F95:H95"/>
-    <mergeCell ref="F86:H86"/>
-    <mergeCell ref="F87:H87"/>
-    <mergeCell ref="F88:H88"/>
-    <mergeCell ref="F89:H89"/>
-    <mergeCell ref="F90:H90"/>
-    <mergeCell ref="F81:H81"/>
-    <mergeCell ref="F82:H82"/>
-    <mergeCell ref="F83:H83"/>
-    <mergeCell ref="F84:H84"/>
-    <mergeCell ref="F85:H85"/>
-    <mergeCell ref="F76:H76"/>
-    <mergeCell ref="F77:H77"/>
-    <mergeCell ref="F78:H78"/>
-    <mergeCell ref="F79:H79"/>
-    <mergeCell ref="F80:H80"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="F74:H74"/>
-    <mergeCell ref="F75:H75"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
@@ -2523,6 +3311,96 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:F2"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="F48:H48"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="F69:H69"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="F76:H76"/>
+    <mergeCell ref="F77:H77"/>
+    <mergeCell ref="F78:H78"/>
+    <mergeCell ref="F79:H79"/>
+    <mergeCell ref="F80:H80"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="F73:H73"/>
+    <mergeCell ref="F74:H74"/>
+    <mergeCell ref="F75:H75"/>
+    <mergeCell ref="F86:H86"/>
+    <mergeCell ref="F87:H87"/>
+    <mergeCell ref="F88:H88"/>
+    <mergeCell ref="F89:H89"/>
+    <mergeCell ref="F90:H90"/>
+    <mergeCell ref="F81:H81"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="F83:H83"/>
+    <mergeCell ref="F84:H84"/>
+    <mergeCell ref="F85:H85"/>
+    <mergeCell ref="F96:H96"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="F98:H98"/>
+    <mergeCell ref="F99:H99"/>
+    <mergeCell ref="F100:H100"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="F93:H93"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="F95:H95"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.47222222222222221" right="0.56944444444444442" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2539,8 +3417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2555,77 +3433,85 @@
       <c r="A1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="58"/>
     </row>
     <row r="2" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="60"/>
     </row>
     <row r="3" spans="1:5" ht="135.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="61"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="62"/>
     </row>
     <row r="4" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="66"/>
+      <c r="B4" s="65">
+        <v>300</v>
+      </c>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="67"/>
     </row>
     <row r="5" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="61"/>
+      <c r="B5" s="61" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="62"/>
     </row>
     <row r="6" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="61"/>
+      <c r="B6" s="61">
+        <v>2</v>
+      </c>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="62"/>
     </row>
     <row r="7" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="64"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="66"/>
+      <c r="B7" s="65">
+        <v>6</v>
+      </c>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="67"/>
     </row>
     <row r="8" spans="1:5" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="63"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2653,7 +3539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B4" sqref="B4:G4"/>
     </sheetView>
   </sheetViews>
@@ -2666,200 +3552,200 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="69"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="70"/>
     </row>
     <row r="2" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="70">
+      <c r="B2" s="79">
         <v>41673</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="62"/>
     </row>
     <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="62"/>
     </row>
     <row r="4" spans="1:7" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="62"/>
     </row>
     <row r="5" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="64"/>
     </row>
     <row r="6" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="68"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="69"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="70"/>
     </row>
     <row r="8" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="72"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="76"/>
     </row>
     <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="61"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="62"/>
     </row>
     <row r="10" spans="1:7" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="61"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="62"/>
     </row>
     <row r="11" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="73"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="74"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="78"/>
     </row>
     <row r="12" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="67" t="s">
+      <c r="A14" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="68"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="69"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="70"/>
     </row>
     <row r="15" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="75"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="76"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="71"/>
+      <c r="G15" s="72"/>
     </row>
     <row r="16" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="61"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="62"/>
     </row>
     <row r="17" spans="1:7" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="60"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="61"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="62"/>
     </row>
     <row r="18" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="77"/>
-      <c r="C18" s="77"/>
-      <c r="D18" s="77"/>
-      <c r="E18" s="77"/>
-      <c r="F18" s="77"/>
-      <c r="G18" s="78"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="74"/>
     </row>
     <row r="19" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:7" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="B15:G15"/>
     <mergeCell ref="B16:G16"/>
     <mergeCell ref="B17:G17"/>
     <mergeCell ref="B18:G18"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
small changes during analysis that hopefully didn't overwrite the original information
</commit_message>
<xml_diff>
--- a/CH_020314_C.xlsx
+++ b/CH_020314_C.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glickfeld_lab\Documents\GitHub\docubase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glickfeld_lab\Documents\docubase\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -62,9 +62,6 @@
     <t>General Info</t>
   </si>
   <si>
-    <t>Ra</t>
-  </si>
-  <si>
     <t>Vrest</t>
   </si>
   <si>
@@ -483,6 +480,9 @@
   </si>
   <si>
     <t>4% PFA</t>
+  </si>
+  <si>
+    <t>Slice</t>
   </si>
 </sst>
 </file>
@@ -1125,15 +1125,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1143,6 +1134,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1233,32 +1233,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1625,15 +1625,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1649,7 +1649,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1657,20 +1657,20 @@
         <v>3</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="147.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="38.1" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B7" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1680,7 +1680,7 @@
     </row>
     <row r="9" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1688,7 +1688,7 @@
     </row>
     <row r="11" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1711,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51:H51"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1734,13 +1734,13 @@
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="55" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D1" s="56"/>
       <c r="E1" s="56"/>
       <c r="F1" s="56"/>
       <c r="G1" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1" s="22">
         <v>297</v>
@@ -1751,14 +1751,14 @@
         <v>8</v>
       </c>
       <c r="B2" s="52"/>
-      <c r="C2" s="38" t="s">
-        <v>149</v>
-      </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="C2" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H2" s="24">
         <v>303</v>
@@ -1772,9 +1772,9 @@
       <c r="C3" s="42">
         <v>34</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
       <c r="G3" s="43"/>
       <c r="H3" s="44"/>
     </row>
@@ -1784,7 +1784,7 @@
       </c>
       <c r="B4" s="54"/>
       <c r="C4" s="45" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D4" s="46"/>
       <c r="E4" s="46"/>
@@ -1804,7 +1804,7 @@
     </row>
     <row r="6" spans="1:8" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>4</v>
@@ -1813,76 +1813,76 @@
         <v>5</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="37"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="40"/>
     </row>
     <row r="7" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="34">
         <v>6</v>
       </c>
       <c r="E7" s="34"/>
-      <c r="F7" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="39"/>
-      <c r="H7" s="40"/>
+      <c r="F7" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="36"/>
+      <c r="H7" s="37"/>
     </row>
     <row r="8" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="34">
         <v>6</v>
       </c>
       <c r="E8" s="34"/>
-      <c r="F8" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="39"/>
-      <c r="H8" s="40"/>
+      <c r="F8" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
     </row>
     <row r="9" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="34">
         <v>6</v>
       </c>
       <c r="E9" s="34"/>
-      <c r="F9" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="39"/>
-      <c r="H9" s="40"/>
+      <c r="F9" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="36"/>
+      <c r="H9" s="37"/>
     </row>
     <row r="10" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -1890,19 +1890,19 @@
       <c r="C10" s="4"/>
       <c r="D10" s="34"/>
       <c r="E10" s="34"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="40"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="37"/>
     </row>
     <row r="11" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>2</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="D11" s="34">
         <v>6</v>
@@ -1910,371 +1910,371 @@
       <c r="E11" s="34">
         <v>-70</v>
       </c>
-      <c r="F11" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="39"/>
-      <c r="H11" s="40"/>
+      <c r="F11" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="36"/>
+      <c r="H11" s="37"/>
     </row>
     <row r="12" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>2</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="34">
         <v>6</v>
       </c>
       <c r="E12" s="34"/>
-      <c r="F12" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="39"/>
-      <c r="H12" s="40"/>
+      <c r="F12" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="36"/>
+      <c r="H12" s="37"/>
     </row>
     <row r="13" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>2</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="34">
         <v>6</v>
       </c>
       <c r="E13" s="34"/>
-      <c r="F13" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" s="39"/>
-      <c r="H13" s="40"/>
+      <c r="F13" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="36"/>
+      <c r="H13" s="37"/>
     </row>
     <row r="14" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>2</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" s="34">
         <v>6</v>
       </c>
       <c r="E14" s="34"/>
-      <c r="F14" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="G14" s="39"/>
-      <c r="H14" s="40"/>
+      <c r="F14" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="36"/>
+      <c r="H14" s="37"/>
     </row>
     <row r="15" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>2</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" s="34">
         <v>6</v>
       </c>
       <c r="E15" s="34"/>
-      <c r="F15" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15" s="39"/>
-      <c r="H15" s="40"/>
+      <c r="F15" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="36"/>
+      <c r="H15" s="37"/>
     </row>
     <row r="16" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>2</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="34">
         <v>6</v>
       </c>
       <c r="E16" s="34"/>
-      <c r="F16" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="39"/>
-      <c r="H16" s="40"/>
+      <c r="F16" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="36"/>
+      <c r="H16" s="37"/>
     </row>
     <row r="17" spans="1:8" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>2</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" s="34">
         <v>6</v>
       </c>
       <c r="E17" s="34"/>
-      <c r="F17" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="G17" s="39"/>
-      <c r="H17" s="40"/>
+      <c r="F17" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="36"/>
+      <c r="H17" s="37"/>
     </row>
     <row r="18" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>2</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" s="34">
         <v>6</v>
       </c>
       <c r="E18" s="34"/>
-      <c r="F18" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="G18" s="39"/>
-      <c r="H18" s="40"/>
+      <c r="F18" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
     </row>
     <row r="19" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>2</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19" s="34">
         <v>6</v>
       </c>
       <c r="E19" s="34"/>
-      <c r="F19" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="G19" s="39"/>
-      <c r="H19" s="40"/>
+      <c r="F19" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="36"/>
+      <c r="H19" s="37"/>
     </row>
     <row r="20" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>2</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" s="34">
         <v>6</v>
       </c>
       <c r="E20" s="34"/>
-      <c r="F20" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="G20" s="39"/>
-      <c r="H20" s="40"/>
+      <c r="F20" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="36"/>
+      <c r="H20" s="37"/>
     </row>
     <row r="21" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>2</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="34">
         <v>6</v>
       </c>
       <c r="E21" s="34"/>
-      <c r="F21" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="G21" s="39"/>
-      <c r="H21" s="40"/>
+      <c r="F21" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" s="36"/>
+      <c r="H21" s="37"/>
     </row>
     <row r="22" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>2</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="34">
         <v>6</v>
       </c>
       <c r="E22" s="34"/>
-      <c r="F22" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="G22" s="39"/>
-      <c r="H22" s="40"/>
+      <c r="F22" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="36"/>
+      <c r="H22" s="37"/>
     </row>
     <row r="23" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>2</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23" s="34">
         <v>6</v>
       </c>
       <c r="E23" s="34"/>
-      <c r="F23" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="G23" s="39"/>
-      <c r="H23" s="40"/>
+      <c r="F23" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23" s="36"/>
+      <c r="H23" s="37"/>
     </row>
     <row r="24" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>2</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24" s="34">
         <v>6</v>
       </c>
       <c r="E24" s="34"/>
-      <c r="F24" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="G24" s="39"/>
-      <c r="H24" s="40"/>
+      <c r="F24" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" s="36"/>
+      <c r="H24" s="37"/>
     </row>
     <row r="25" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>2</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D25" s="34">
         <v>6</v>
       </c>
       <c r="E25" s="34"/>
-      <c r="F25" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="G25" s="39"/>
-      <c r="H25" s="40"/>
+      <c r="F25" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="G25" s="36"/>
+      <c r="H25" s="37"/>
     </row>
     <row r="26" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>2</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D26" s="34">
         <v>6</v>
       </c>
       <c r="E26" s="34"/>
-      <c r="F26" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="G26" s="39"/>
-      <c r="H26" s="40"/>
+      <c r="F26" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" s="36"/>
+      <c r="H26" s="37"/>
     </row>
     <row r="27" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>2</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D27" s="34">
         <v>6</v>
       </c>
       <c r="E27" s="34"/>
-      <c r="F27" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="G27" s="39"/>
-      <c r="H27" s="40"/>
+      <c r="F27" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" s="36"/>
+      <c r="H27" s="37"/>
     </row>
     <row r="28" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>2</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D28" s="34">
         <v>6</v>
       </c>
       <c r="E28" s="34"/>
-      <c r="F28" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="G28" s="39"/>
-      <c r="H28" s="40"/>
+      <c r="F28" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="G28" s="36"/>
+      <c r="H28" s="37"/>
     </row>
     <row r="29" spans="1:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>2</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D29" s="34">
         <v>6</v>
       </c>
       <c r="E29" s="34"/>
-      <c r="F29" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="G29" s="39"/>
-      <c r="H29" s="40"/>
+      <c r="F29" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" s="36"/>
+      <c r="H29" s="37"/>
     </row>
     <row r="30" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
@@ -2286,13 +2286,13 @@
         <v>6</v>
       </c>
       <c r="E30" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="F30" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="G30" s="39"/>
-      <c r="H30" s="40"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="37"/>
     </row>
     <row r="31" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
@@ -2300,19 +2300,19 @@
       <c r="C31" s="4"/>
       <c r="D31" s="34"/>
       <c r="E31" s="34"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="40"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="37"/>
     </row>
     <row r="32" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>3</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D32" s="34">
         <v>9</v>
@@ -2320,291 +2320,291 @@
       <c r="E32" s="34">
         <v>-75</v>
       </c>
-      <c r="F32" s="38" t="s">
-        <v>90</v>
-      </c>
-      <c r="G32" s="39"/>
-      <c r="H32" s="40"/>
+      <c r="F32" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="G32" s="36"/>
+      <c r="H32" s="37"/>
     </row>
     <row r="33" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>3</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D33" s="34">
         <v>9</v>
       </c>
       <c r="E33" s="34"/>
-      <c r="F33" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="G33" s="39"/>
-      <c r="H33" s="40"/>
+      <c r="F33" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="G33" s="36"/>
+      <c r="H33" s="37"/>
     </row>
     <row r="34" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>3</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D34" s="34">
         <v>9</v>
       </c>
       <c r="E34" s="34"/>
-      <c r="F34" s="38" t="s">
-        <v>94</v>
-      </c>
-      <c r="G34" s="39"/>
-      <c r="H34" s="40"/>
+      <c r="F34" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="G34" s="36"/>
+      <c r="H34" s="37"/>
     </row>
     <row r="35" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>3</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D35" s="34">
         <v>9</v>
       </c>
       <c r="E35" s="34"/>
-      <c r="F35" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="G35" s="39"/>
-      <c r="H35" s="40"/>
+      <c r="F35" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="G35" s="36"/>
+      <c r="H35" s="37"/>
     </row>
     <row r="36" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>3</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D36" s="34">
         <v>9</v>
       </c>
       <c r="E36" s="34"/>
-      <c r="F36" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="G36" s="39"/>
-      <c r="H36" s="40"/>
+      <c r="F36" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="G36" s="36"/>
+      <c r="H36" s="37"/>
     </row>
     <row r="37" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>3</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D37" s="34">
         <v>9</v>
       </c>
       <c r="E37" s="34"/>
-      <c r="F37" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="G37" s="39"/>
-      <c r="H37" s="40"/>
+      <c r="F37" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="G37" s="36"/>
+      <c r="H37" s="37"/>
     </row>
     <row r="38" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>3</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D38" s="34">
         <v>9</v>
       </c>
       <c r="E38" s="34"/>
-      <c r="F38" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="G38" s="39"/>
-      <c r="H38" s="40"/>
+      <c r="F38" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="G38" s="36"/>
+      <c r="H38" s="37"/>
     </row>
     <row r="39" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>3</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D39" s="34">
         <v>9</v>
       </c>
       <c r="E39" s="34"/>
-      <c r="F39" s="38" t="s">
-        <v>104</v>
-      </c>
-      <c r="G39" s="39"/>
-      <c r="H39" s="40"/>
+      <c r="F39" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="G39" s="36"/>
+      <c r="H39" s="37"/>
     </row>
     <row r="40" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>3</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D40" s="34">
         <v>9</v>
       </c>
       <c r="E40" s="34"/>
-      <c r="F40" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="G40" s="39"/>
-      <c r="H40" s="40"/>
+      <c r="F40" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="G40" s="36"/>
+      <c r="H40" s="37"/>
     </row>
     <row r="41" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>3</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D41" s="34">
         <v>9</v>
       </c>
       <c r="E41" s="34"/>
-      <c r="F41" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="G41" s="39"/>
-      <c r="H41" s="40"/>
+      <c r="F41" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="G41" s="36"/>
+      <c r="H41" s="37"/>
     </row>
     <row r="42" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>3</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D42" s="34">
         <v>9</v>
       </c>
       <c r="E42" s="34"/>
-      <c r="F42" s="38" t="s">
-        <v>110</v>
-      </c>
-      <c r="G42" s="39"/>
-      <c r="H42" s="40"/>
+      <c r="F42" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="G42" s="36"/>
+      <c r="H42" s="37"/>
     </row>
     <row r="43" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>3</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D43" s="34">
         <v>9</v>
       </c>
       <c r="E43" s="34"/>
-      <c r="F43" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="G43" s="39"/>
-      <c r="H43" s="40"/>
+      <c r="F43" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="G43" s="36"/>
+      <c r="H43" s="37"/>
     </row>
     <row r="44" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>3</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D44" s="34">
         <v>9</v>
       </c>
       <c r="E44" s="34"/>
-      <c r="F44" s="38" t="s">
-        <v>114</v>
-      </c>
-      <c r="G44" s="39"/>
-      <c r="H44" s="40"/>
+      <c r="F44" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="G44" s="36"/>
+      <c r="H44" s="37"/>
     </row>
     <row r="45" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>3</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D45" s="34">
         <v>9</v>
       </c>
       <c r="E45" s="34"/>
-      <c r="F45" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="G45" s="39"/>
-      <c r="H45" s="40"/>
+      <c r="F45" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="G45" s="36"/>
+      <c r="H45" s="37"/>
     </row>
     <row r="46" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>3</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D46" s="34">
         <v>9</v>
       </c>
       <c r="E46" s="34"/>
-      <c r="F46" s="38" t="s">
-        <v>118</v>
-      </c>
-      <c r="G46" s="39"/>
-      <c r="H46" s="40"/>
+      <c r="F46" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="G46" s="36"/>
+      <c r="H46" s="37"/>
     </row>
     <row r="47" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
@@ -2614,13 +2614,13 @@
       <c r="C47" s="4"/>
       <c r="D47" s="34"/>
       <c r="E47" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="F47" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="G47" s="39"/>
-      <c r="H47" s="40"/>
+        <v>86</v>
+      </c>
+      <c r="F47" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="G47" s="36"/>
+      <c r="H47" s="37"/>
     </row>
     <row r="48" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
@@ -2628,19 +2628,19 @@
       <c r="C48" s="4"/>
       <c r="D48" s="34"/>
       <c r="E48" s="34"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="40"/>
+      <c r="F48" s="35"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="37"/>
     </row>
     <row r="49" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>4</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D49" s="34">
         <v>9</v>
@@ -2648,271 +2648,271 @@
       <c r="E49" s="34">
         <v>-65</v>
       </c>
-      <c r="F49" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="G49" s="39"/>
-      <c r="H49" s="40"/>
+      <c r="F49" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="G49" s="36"/>
+      <c r="H49" s="37"/>
     </row>
     <row r="50" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>4</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D50" s="34">
         <v>9</v>
       </c>
       <c r="E50" s="34"/>
-      <c r="F50" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="G50" s="39"/>
-      <c r="H50" s="40"/>
+      <c r="F50" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="G50" s="36"/>
+      <c r="H50" s="37"/>
     </row>
     <row r="51" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>4</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D51" s="34">
         <v>9</v>
       </c>
       <c r="E51" s="34"/>
-      <c r="F51" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="G51" s="39"/>
-      <c r="H51" s="40"/>
+      <c r="F51" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="G51" s="36"/>
+      <c r="H51" s="37"/>
     </row>
     <row r="52" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>4</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D52" s="34">
         <v>9</v>
       </c>
       <c r="E52" s="34"/>
-      <c r="F52" s="38" t="s">
-        <v>127</v>
-      </c>
-      <c r="G52" s="39"/>
-      <c r="H52" s="40"/>
+      <c r="F52" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="G52" s="36"/>
+      <c r="H52" s="37"/>
     </row>
     <row r="53" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>4</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D53" s="34">
         <v>9</v>
       </c>
       <c r="E53" s="34"/>
-      <c r="F53" s="38" t="s">
-        <v>129</v>
-      </c>
-      <c r="G53" s="39"/>
-      <c r="H53" s="40"/>
+      <c r="F53" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="G53" s="36"/>
+      <c r="H53" s="37"/>
     </row>
     <row r="54" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>4</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D54" s="34">
         <v>9</v>
       </c>
       <c r="E54" s="34"/>
-      <c r="F54" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="G54" s="39"/>
-      <c r="H54" s="40"/>
+      <c r="F54" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="G54" s="36"/>
+      <c r="H54" s="37"/>
     </row>
     <row r="55" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>4</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D55" s="34">
         <v>9</v>
       </c>
       <c r="E55" s="34"/>
-      <c r="F55" s="38" t="s">
-        <v>133</v>
-      </c>
-      <c r="G55" s="39"/>
-      <c r="H55" s="40"/>
+      <c r="F55" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="G55" s="36"/>
+      <c r="H55" s="37"/>
     </row>
     <row r="56" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>4</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D56" s="34">
         <v>9</v>
       </c>
       <c r="E56" s="34"/>
-      <c r="F56" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="G56" s="39"/>
-      <c r="H56" s="40"/>
+      <c r="F56" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="G56" s="36"/>
+      <c r="H56" s="37"/>
     </row>
     <row r="57" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>4</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D57" s="34">
         <v>9</v>
       </c>
       <c r="E57" s="34"/>
-      <c r="F57" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="G57" s="39"/>
-      <c r="H57" s="40"/>
+      <c r="F57" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="G57" s="36"/>
+      <c r="H57" s="37"/>
     </row>
     <row r="58" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>4</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D58" s="34">
         <v>9</v>
       </c>
       <c r="E58" s="34"/>
-      <c r="F58" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="G58" s="39"/>
-      <c r="H58" s="40"/>
+      <c r="F58" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="G58" s="36"/>
+      <c r="H58" s="37"/>
     </row>
     <row r="59" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>4</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D59" s="34">
         <v>9</v>
       </c>
       <c r="E59" s="34"/>
-      <c r="F59" s="38" t="s">
-        <v>141</v>
-      </c>
-      <c r="G59" s="39"/>
-      <c r="H59" s="40"/>
+      <c r="F59" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="G59" s="36"/>
+      <c r="H59" s="37"/>
     </row>
     <row r="60" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>4</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D60" s="34">
         <v>9</v>
       </c>
       <c r="E60" s="34"/>
-      <c r="F60" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="G60" s="39"/>
-      <c r="H60" s="40"/>
+      <c r="F60" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="G60" s="36"/>
+      <c r="H60" s="37"/>
     </row>
     <row r="61" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>4</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D61" s="34">
         <v>9</v>
       </c>
       <c r="E61" s="34"/>
-      <c r="F61" s="38" t="s">
-        <v>145</v>
-      </c>
-      <c r="G61" s="39"/>
-      <c r="H61" s="40"/>
+      <c r="F61" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="G61" s="36"/>
+      <c r="H61" s="37"/>
     </row>
     <row r="62" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>4</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="34">
         <v>9</v>
       </c>
       <c r="E62" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="F62" s="38" t="s">
-        <v>147</v>
-      </c>
-      <c r="G62" s="39"/>
-      <c r="H62" s="40"/>
+        <v>86</v>
+      </c>
+      <c r="F62" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="G62" s="36"/>
+      <c r="H62" s="37"/>
     </row>
     <row r="63" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
@@ -2920,9 +2920,9 @@
       <c r="C63" s="4"/>
       <c r="D63" s="5"/>
       <c r="E63" s="23"/>
-      <c r="F63" s="38"/>
-      <c r="G63" s="39"/>
-      <c r="H63" s="40"/>
+      <c r="F63" s="35"/>
+      <c r="G63" s="36"/>
+      <c r="H63" s="37"/>
     </row>
     <row r="64" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
@@ -2930,9 +2930,9 @@
       <c r="C64" s="4"/>
       <c r="D64" s="5"/>
       <c r="E64" s="23"/>
-      <c r="F64" s="38"/>
-      <c r="G64" s="39"/>
-      <c r="H64" s="40"/>
+      <c r="F64" s="35"/>
+      <c r="G64" s="36"/>
+      <c r="H64" s="37"/>
     </row>
     <row r="65" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
@@ -2940,9 +2940,9 @@
       <c r="C65" s="4"/>
       <c r="D65" s="5"/>
       <c r="E65" s="23"/>
-      <c r="F65" s="38"/>
-      <c r="G65" s="39"/>
-      <c r="H65" s="40"/>
+      <c r="F65" s="35"/>
+      <c r="G65" s="36"/>
+      <c r="H65" s="37"/>
     </row>
     <row r="66" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
@@ -2950,9 +2950,9 @@
       <c r="C66" s="4"/>
       <c r="D66" s="5"/>
       <c r="E66" s="23"/>
-      <c r="F66" s="38"/>
-      <c r="G66" s="39"/>
-      <c r="H66" s="40"/>
+      <c r="F66" s="35"/>
+      <c r="G66" s="36"/>
+      <c r="H66" s="37"/>
     </row>
     <row r="67" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
@@ -2960,9 +2960,9 @@
       <c r="C67" s="4"/>
       <c r="D67" s="5"/>
       <c r="E67" s="23"/>
-      <c r="F67" s="38"/>
-      <c r="G67" s="39"/>
-      <c r="H67" s="40"/>
+      <c r="F67" s="35"/>
+      <c r="G67" s="36"/>
+      <c r="H67" s="37"/>
     </row>
     <row r="68" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
@@ -2970,9 +2970,9 @@
       <c r="C68" s="4"/>
       <c r="D68" s="5"/>
       <c r="E68" s="23"/>
-      <c r="F68" s="38"/>
-      <c r="G68" s="39"/>
-      <c r="H68" s="40"/>
+      <c r="F68" s="35"/>
+      <c r="G68" s="36"/>
+      <c r="H68" s="37"/>
     </row>
     <row r="69" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
@@ -2980,9 +2980,9 @@
       <c r="C69" s="4"/>
       <c r="D69" s="5"/>
       <c r="E69" s="23"/>
-      <c r="F69" s="38"/>
-      <c r="G69" s="39"/>
-      <c r="H69" s="40"/>
+      <c r="F69" s="35"/>
+      <c r="G69" s="36"/>
+      <c r="H69" s="37"/>
     </row>
     <row r="70" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
@@ -2990,9 +2990,9 @@
       <c r="C70" s="4"/>
       <c r="D70" s="5"/>
       <c r="E70" s="23"/>
-      <c r="F70" s="38"/>
-      <c r="G70" s="39"/>
-      <c r="H70" s="40"/>
+      <c r="F70" s="35"/>
+      <c r="G70" s="36"/>
+      <c r="H70" s="37"/>
     </row>
     <row r="71" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
@@ -3000,9 +3000,9 @@
       <c r="C71" s="4"/>
       <c r="D71" s="5"/>
       <c r="E71" s="23"/>
-      <c r="F71" s="38"/>
-      <c r="G71" s="39"/>
-      <c r="H71" s="40"/>
+      <c r="F71" s="35"/>
+      <c r="G71" s="36"/>
+      <c r="H71" s="37"/>
     </row>
     <row r="72" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
@@ -3010,9 +3010,9 @@
       <c r="C72" s="4"/>
       <c r="D72" s="5"/>
       <c r="E72" s="23"/>
-      <c r="F72" s="38"/>
-      <c r="G72" s="39"/>
-      <c r="H72" s="40"/>
+      <c r="F72" s="35"/>
+      <c r="G72" s="36"/>
+      <c r="H72" s="37"/>
     </row>
     <row r="73" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
@@ -3020,9 +3020,9 @@
       <c r="C73" s="4"/>
       <c r="D73" s="5"/>
       <c r="E73" s="23"/>
-      <c r="F73" s="38"/>
-      <c r="G73" s="39"/>
-      <c r="H73" s="40"/>
+      <c r="F73" s="35"/>
+      <c r="G73" s="36"/>
+      <c r="H73" s="37"/>
     </row>
     <row r="74" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
@@ -3030,9 +3030,9 @@
       <c r="C74" s="4"/>
       <c r="D74" s="5"/>
       <c r="E74" s="23"/>
-      <c r="F74" s="38"/>
-      <c r="G74" s="39"/>
-      <c r="H74" s="40"/>
+      <c r="F74" s="35"/>
+      <c r="G74" s="36"/>
+      <c r="H74" s="37"/>
     </row>
     <row r="75" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
@@ -3040,9 +3040,9 @@
       <c r="C75" s="4"/>
       <c r="D75" s="5"/>
       <c r="E75" s="23"/>
-      <c r="F75" s="38"/>
-      <c r="G75" s="39"/>
-      <c r="H75" s="40"/>
+      <c r="F75" s="35"/>
+      <c r="G75" s="36"/>
+      <c r="H75" s="37"/>
     </row>
     <row r="76" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
@@ -3050,9 +3050,9 @@
       <c r="C76" s="4"/>
       <c r="D76" s="5"/>
       <c r="E76" s="23"/>
-      <c r="F76" s="38"/>
-      <c r="G76" s="39"/>
-      <c r="H76" s="40"/>
+      <c r="F76" s="35"/>
+      <c r="G76" s="36"/>
+      <c r="H76" s="37"/>
     </row>
     <row r="77" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
@@ -3060,9 +3060,9 @@
       <c r="C77" s="4"/>
       <c r="D77" s="5"/>
       <c r="E77" s="23"/>
-      <c r="F77" s="38"/>
-      <c r="G77" s="39"/>
-      <c r="H77" s="40"/>
+      <c r="F77" s="35"/>
+      <c r="G77" s="36"/>
+      <c r="H77" s="37"/>
     </row>
     <row r="78" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
@@ -3070,9 +3070,9 @@
       <c r="C78" s="4"/>
       <c r="D78" s="5"/>
       <c r="E78" s="23"/>
-      <c r="F78" s="38"/>
-      <c r="G78" s="39"/>
-      <c r="H78" s="40"/>
+      <c r="F78" s="35"/>
+      <c r="G78" s="36"/>
+      <c r="H78" s="37"/>
     </row>
     <row r="79" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
@@ -3080,9 +3080,9 @@
       <c r="C79" s="4"/>
       <c r="D79" s="5"/>
       <c r="E79" s="23"/>
-      <c r="F79" s="38"/>
-      <c r="G79" s="39"/>
-      <c r="H79" s="40"/>
+      <c r="F79" s="35"/>
+      <c r="G79" s="36"/>
+      <c r="H79" s="37"/>
     </row>
     <row r="80" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
@@ -3090,9 +3090,9 @@
       <c r="C80" s="4"/>
       <c r="D80" s="5"/>
       <c r="E80" s="23"/>
-      <c r="F80" s="38"/>
-      <c r="G80" s="39"/>
-      <c r="H80" s="40"/>
+      <c r="F80" s="35"/>
+      <c r="G80" s="36"/>
+      <c r="H80" s="37"/>
     </row>
     <row r="81" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
@@ -3100,9 +3100,9 @@
       <c r="C81" s="4"/>
       <c r="D81" s="5"/>
       <c r="E81" s="23"/>
-      <c r="F81" s="38"/>
-      <c r="G81" s="39"/>
-      <c r="H81" s="40"/>
+      <c r="F81" s="35"/>
+      <c r="G81" s="36"/>
+      <c r="H81" s="37"/>
     </row>
     <row r="82" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
@@ -3110,9 +3110,9 @@
       <c r="C82" s="4"/>
       <c r="D82" s="5"/>
       <c r="E82" s="23"/>
-      <c r="F82" s="38"/>
-      <c r="G82" s="39"/>
-      <c r="H82" s="40"/>
+      <c r="F82" s="35"/>
+      <c r="G82" s="36"/>
+      <c r="H82" s="37"/>
     </row>
     <row r="83" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
@@ -3120,9 +3120,9 @@
       <c r="C83" s="4"/>
       <c r="D83" s="5"/>
       <c r="E83" s="23"/>
-      <c r="F83" s="38"/>
-      <c r="G83" s="39"/>
-      <c r="H83" s="40"/>
+      <c r="F83" s="35"/>
+      <c r="G83" s="36"/>
+      <c r="H83" s="37"/>
     </row>
     <row r="84" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
@@ -3130,9 +3130,9 @@
       <c r="C84" s="4"/>
       <c r="D84" s="5"/>
       <c r="E84" s="23"/>
-      <c r="F84" s="38"/>
-      <c r="G84" s="39"/>
-      <c r="H84" s="40"/>
+      <c r="F84" s="35"/>
+      <c r="G84" s="36"/>
+      <c r="H84" s="37"/>
     </row>
     <row r="85" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
@@ -3140,9 +3140,9 @@
       <c r="C85" s="4"/>
       <c r="D85" s="5"/>
       <c r="E85" s="23"/>
-      <c r="F85" s="38"/>
-      <c r="G85" s="39"/>
-      <c r="H85" s="40"/>
+      <c r="F85" s="35"/>
+      <c r="G85" s="36"/>
+      <c r="H85" s="37"/>
     </row>
     <row r="86" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
@@ -3150,9 +3150,9 @@
       <c r="C86" s="4"/>
       <c r="D86" s="5"/>
       <c r="E86" s="23"/>
-      <c r="F86" s="38"/>
-      <c r="G86" s="39"/>
-      <c r="H86" s="40"/>
+      <c r="F86" s="35"/>
+      <c r="G86" s="36"/>
+      <c r="H86" s="37"/>
     </row>
     <row r="87" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
@@ -3160,9 +3160,9 @@
       <c r="C87" s="4"/>
       <c r="D87" s="5"/>
       <c r="E87" s="23"/>
-      <c r="F87" s="38"/>
-      <c r="G87" s="39"/>
-      <c r="H87" s="40"/>
+      <c r="F87" s="35"/>
+      <c r="G87" s="36"/>
+      <c r="H87" s="37"/>
     </row>
     <row r="88" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
@@ -3170,9 +3170,9 @@
       <c r="C88" s="4"/>
       <c r="D88" s="5"/>
       <c r="E88" s="23"/>
-      <c r="F88" s="38"/>
-      <c r="G88" s="39"/>
-      <c r="H88" s="40"/>
+      <c r="F88" s="35"/>
+      <c r="G88" s="36"/>
+      <c r="H88" s="37"/>
     </row>
     <row r="89" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
@@ -3180,9 +3180,9 @@
       <c r="C89" s="4"/>
       <c r="D89" s="5"/>
       <c r="E89" s="23"/>
-      <c r="F89" s="38"/>
-      <c r="G89" s="39"/>
-      <c r="H89" s="40"/>
+      <c r="F89" s="35"/>
+      <c r="G89" s="36"/>
+      <c r="H89" s="37"/>
     </row>
     <row r="90" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
@@ -3190,9 +3190,9 @@
       <c r="C90" s="4"/>
       <c r="D90" s="5"/>
       <c r="E90" s="23"/>
-      <c r="F90" s="38"/>
-      <c r="G90" s="39"/>
-      <c r="H90" s="40"/>
+      <c r="F90" s="35"/>
+      <c r="G90" s="36"/>
+      <c r="H90" s="37"/>
     </row>
     <row r="91" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
@@ -3200,9 +3200,9 @@
       <c r="C91" s="4"/>
       <c r="D91" s="5"/>
       <c r="E91" s="23"/>
-      <c r="F91" s="38"/>
-      <c r="G91" s="39"/>
-      <c r="H91" s="40"/>
+      <c r="F91" s="35"/>
+      <c r="G91" s="36"/>
+      <c r="H91" s="37"/>
     </row>
     <row r="92" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
@@ -3210,9 +3210,9 @@
       <c r="C92" s="4"/>
       <c r="D92" s="5"/>
       <c r="E92" s="23"/>
-      <c r="F92" s="38"/>
-      <c r="G92" s="39"/>
-      <c r="H92" s="40"/>
+      <c r="F92" s="35"/>
+      <c r="G92" s="36"/>
+      <c r="H92" s="37"/>
     </row>
     <row r="93" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
@@ -3220,9 +3220,9 @@
       <c r="C93" s="4"/>
       <c r="D93" s="5"/>
       <c r="E93" s="23"/>
-      <c r="F93" s="38"/>
-      <c r="G93" s="39"/>
-      <c r="H93" s="40"/>
+      <c r="F93" s="35"/>
+      <c r="G93" s="36"/>
+      <c r="H93" s="37"/>
     </row>
     <row r="94" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
@@ -3230,9 +3230,9 @@
       <c r="C94" s="4"/>
       <c r="D94" s="5"/>
       <c r="E94" s="23"/>
-      <c r="F94" s="38"/>
-      <c r="G94" s="39"/>
-      <c r="H94" s="40"/>
+      <c r="F94" s="35"/>
+      <c r="G94" s="36"/>
+      <c r="H94" s="37"/>
     </row>
     <row r="95" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
@@ -3240,9 +3240,9 @@
       <c r="C95" s="4"/>
       <c r="D95" s="5"/>
       <c r="E95" s="23"/>
-      <c r="F95" s="38"/>
-      <c r="G95" s="39"/>
-      <c r="H95" s="40"/>
+      <c r="F95" s="35"/>
+      <c r="G95" s="36"/>
+      <c r="H95" s="37"/>
     </row>
     <row r="96" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
@@ -3250,9 +3250,9 @@
       <c r="C96" s="4"/>
       <c r="D96" s="5"/>
       <c r="E96" s="23"/>
-      <c r="F96" s="38"/>
-      <c r="G96" s="39"/>
-      <c r="H96" s="40"/>
+      <c r="F96" s="35"/>
+      <c r="G96" s="36"/>
+      <c r="H96" s="37"/>
     </row>
     <row r="97" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
@@ -3260,9 +3260,9 @@
       <c r="C97" s="4"/>
       <c r="D97" s="5"/>
       <c r="E97" s="23"/>
-      <c r="F97" s="38"/>
-      <c r="G97" s="39"/>
-      <c r="H97" s="40"/>
+      <c r="F97" s="35"/>
+      <c r="G97" s="36"/>
+      <c r="H97" s="37"/>
     </row>
     <row r="98" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
@@ -3270,9 +3270,9 @@
       <c r="C98" s="4"/>
       <c r="D98" s="5"/>
       <c r="E98" s="23"/>
-      <c r="F98" s="38"/>
-      <c r="G98" s="39"/>
-      <c r="H98" s="40"/>
+      <c r="F98" s="35"/>
+      <c r="G98" s="36"/>
+      <c r="H98" s="37"/>
     </row>
     <row r="99" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
@@ -3280,9 +3280,9 @@
       <c r="C99" s="4"/>
       <c r="D99" s="5"/>
       <c r="E99" s="23"/>
-      <c r="F99" s="38"/>
-      <c r="G99" s="39"/>
-      <c r="H99" s="40"/>
+      <c r="F99" s="35"/>
+      <c r="G99" s="36"/>
+      <c r="H99" s="37"/>
     </row>
     <row r="100" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
@@ -3290,103 +3290,13 @@
       <c r="C100" s="4"/>
       <c r="D100" s="5"/>
       <c r="E100" s="23"/>
-      <c r="F100" s="38"/>
-      <c r="G100" s="39"/>
-      <c r="H100" s="40"/>
+      <c r="F100" s="35"/>
+      <c r="G100" s="36"/>
+      <c r="H100" s="37"/>
     </row>
     <row r="101" spans="1:8" ht="39" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="F96:H96"/>
-    <mergeCell ref="F97:H97"/>
-    <mergeCell ref="F98:H98"/>
-    <mergeCell ref="F99:H99"/>
-    <mergeCell ref="F100:H100"/>
-    <mergeCell ref="F91:H91"/>
-    <mergeCell ref="F92:H92"/>
-    <mergeCell ref="F93:H93"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="F95:H95"/>
-    <mergeCell ref="F86:H86"/>
-    <mergeCell ref="F87:H87"/>
-    <mergeCell ref="F88:H88"/>
-    <mergeCell ref="F89:H89"/>
-    <mergeCell ref="F90:H90"/>
-    <mergeCell ref="F81:H81"/>
-    <mergeCell ref="F82:H82"/>
-    <mergeCell ref="F83:H83"/>
-    <mergeCell ref="F84:H84"/>
-    <mergeCell ref="F85:H85"/>
-    <mergeCell ref="F76:H76"/>
-    <mergeCell ref="F77:H77"/>
-    <mergeCell ref="F78:H78"/>
-    <mergeCell ref="F79:H79"/>
-    <mergeCell ref="F80:H80"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="F74:H74"/>
-    <mergeCell ref="F75:H75"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
@@ -3401,6 +3311,96 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:F2"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="F48:H48"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="F69:H69"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="F76:H76"/>
+    <mergeCell ref="F77:H77"/>
+    <mergeCell ref="F78:H78"/>
+    <mergeCell ref="F79:H79"/>
+    <mergeCell ref="F80:H80"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="F73:H73"/>
+    <mergeCell ref="F74:H74"/>
+    <mergeCell ref="F75:H75"/>
+    <mergeCell ref="F86:H86"/>
+    <mergeCell ref="F87:H87"/>
+    <mergeCell ref="F88:H88"/>
+    <mergeCell ref="F89:H89"/>
+    <mergeCell ref="F90:H90"/>
+    <mergeCell ref="F81:H81"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="F83:H83"/>
+    <mergeCell ref="F84:H84"/>
+    <mergeCell ref="F85:H85"/>
+    <mergeCell ref="F96:H96"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="F98:H98"/>
+    <mergeCell ref="F99:H99"/>
+    <mergeCell ref="F100:H100"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="F93:H93"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="F95:H95"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.47222222222222221" right="0.56944444444444442" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3431,10 +3431,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="57" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" s="57" t="s">
-        <v>15</v>
       </c>
       <c r="C1" s="57"/>
       <c r="D1" s="57"/>
@@ -3442,10 +3442,10 @@
     </row>
     <row r="2" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="59" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" s="59" t="s">
-        <v>17</v>
       </c>
       <c r="C2" s="59"/>
       <c r="D2" s="59"/>
@@ -3453,7 +3453,7 @@
     </row>
     <row r="3" spans="1:5" ht="135.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="61"/>
       <c r="C3" s="61"/>
@@ -3462,7 +3462,7 @@
     </row>
     <row r="4" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="65">
         <v>300</v>
@@ -3473,10 +3473,10 @@
     </row>
     <row r="5" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="61" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C5" s="61"/>
       <c r="D5" s="61"/>
@@ -3484,7 +3484,7 @@
     </row>
     <row r="6" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="61">
         <v>2</v>
@@ -3495,7 +3495,7 @@
     </row>
     <row r="7" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="65">
         <v>6</v>
@@ -3506,7 +3506,7 @@
     </row>
     <row r="8" spans="1:5" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="63"/>
       <c r="C8" s="63"/>
@@ -3553,7 +3553,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="68" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="69"/>
       <c r="C1" s="69"/>
@@ -3564,9 +3564,9 @@
     </row>
     <row r="2" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="71">
+        <v>23</v>
+      </c>
+      <c r="B2" s="79">
         <v>41673</v>
       </c>
       <c r="C2" s="61"/>
@@ -3577,10 +3577,10 @@
     </row>
     <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="61" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="61"/>
       <c r="D3" s="61"/>
@@ -3593,7 +3593,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="61" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="61"/>
       <c r="D4" s="61"/>
@@ -3603,10 +3603,10 @@
     </row>
     <row r="5" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="63"/>
       <c r="D5" s="63"/>
@@ -3617,7 +3617,7 @@
     <row r="6" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="68" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="69"/>
       <c r="C7" s="69"/>
@@ -3628,18 +3628,18 @@
     </row>
     <row r="8" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="73"/>
+        <v>23</v>
+      </c>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="76"/>
     </row>
     <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="61"/>
       <c r="C9" s="61"/>
@@ -3661,20 +3661,20 @@
     </row>
     <row r="11" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="74"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="75"/>
+        <v>25</v>
+      </c>
+      <c r="B11" s="77"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="78"/>
     </row>
     <row r="12" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="68" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="69"/>
       <c r="C14" s="69"/>
@@ -3685,18 +3685,18 @@
     </row>
     <row r="15" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="76"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="77"/>
+        <v>23</v>
+      </c>
+      <c r="B15" s="71"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="71"/>
+      <c r="G15" s="72"/>
     </row>
     <row r="16" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="61"/>
       <c r="C16" s="61"/>
@@ -3718,34 +3718,34 @@
     </row>
     <row r="18" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="78"/>
-      <c r="C18" s="78"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="78"/>
-      <c r="F18" s="78"/>
-      <c r="G18" s="79"/>
+        <v>25</v>
+      </c>
+      <c r="B18" s="73"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="74"/>
     </row>
     <row r="19" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:7" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="B15:G15"/>
     <mergeCell ref="B16:G16"/>
     <mergeCell ref="B17:G17"/>
     <mergeCell ref="B18:G18"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>